<commit_message>
minor bug in named range
</commit_message>
<xml_diff>
--- a/INLog.xlsx
+++ b/INLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{73480163-FD41-4C42-8920-71C251657E9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36672473-4682-4081-B527-E77B0333438E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8B70657C-29D5-49E6-ACD9-4E39DF125711}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="48">
   <si>
     <t>Date</t>
   </si>
@@ -134,6 +134,51 @@
   </si>
   <si>
     <t>CF (30g)</t>
+  </si>
+  <si>
+    <t>Misc</t>
+  </si>
+  <si>
+    <t>Bundle Packaging</t>
+  </si>
+  <si>
+    <t>test recored 1</t>
+  </si>
+  <si>
+    <t>Tape</t>
+  </si>
+  <si>
+    <t>Cardbox (L)</t>
+  </si>
+  <si>
+    <t>Cardbox (M)</t>
+  </si>
+  <si>
+    <t>Cardbox (S)</t>
+  </si>
+  <si>
+    <t>SC (65g)</t>
+  </si>
+  <si>
+    <t>SC (30g)</t>
+  </si>
+  <si>
+    <t>PH (65g)</t>
+  </si>
+  <si>
+    <t>PH (30g)</t>
+  </si>
+  <si>
+    <t>SC (5KG)</t>
+  </si>
+  <si>
+    <t>SC (330g)</t>
+  </si>
+  <si>
+    <t>PH (5KG)</t>
+  </si>
+  <si>
+    <t>PH (330g)</t>
   </si>
 </sst>
 </file>
@@ -486,10 +531,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6403F870-72AC-41C9-92A2-864504D91BE2}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:G53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53:G106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1175,7 +1220,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>44715.469108796293</v>
       </c>
@@ -1189,7 +1234,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>44715.469097222223</v>
       </c>
@@ -1203,7 +1248,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>44715.469097222223</v>
       </c>
@@ -1217,7 +1262,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>44715.469097222223</v>
       </c>
@@ -1229,6 +1274,924 @@
       </c>
       <c r="E52">
         <v>342</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>44715.759432870371</v>
+      </c>
+      <c r="B53" t="s">
+        <v>33</v>
+      </c>
+      <c r="C53" t="s">
+        <v>34</v>
+      </c>
+      <c r="E53">
+        <v>2432</v>
+      </c>
+      <c r="G53" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>44715.759432870371</v>
+      </c>
+      <c r="B54" t="s">
+        <v>33</v>
+      </c>
+      <c r="C54" t="s">
+        <v>36</v>
+      </c>
+      <c r="E54">
+        <v>56</v>
+      </c>
+      <c r="G54" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>44715.759432870371</v>
+      </c>
+      <c r="B55" t="s">
+        <v>33</v>
+      </c>
+      <c r="C55" t="s">
+        <v>37</v>
+      </c>
+      <c r="E55">
+        <v>5654</v>
+      </c>
+      <c r="G55" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>44715.759432870371</v>
+      </c>
+      <c r="B56" t="s">
+        <v>33</v>
+      </c>
+      <c r="C56" t="s">
+        <v>38</v>
+      </c>
+      <c r="E56">
+        <v>4789</v>
+      </c>
+      <c r="G56" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>44715.759432870371</v>
+      </c>
+      <c r="B57" t="s">
+        <v>33</v>
+      </c>
+      <c r="C57" t="s">
+        <v>39</v>
+      </c>
+      <c r="E57">
+        <v>546</v>
+      </c>
+      <c r="G57" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>44715.759432870371</v>
+      </c>
+      <c r="B58" t="s">
+        <v>9</v>
+      </c>
+      <c r="C58" t="s">
+        <v>40</v>
+      </c>
+      <c r="E58">
+        <v>81</v>
+      </c>
+      <c r="G58" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>44715.759432870371</v>
+      </c>
+      <c r="B59" t="s">
+        <v>9</v>
+      </c>
+      <c r="C59" t="s">
+        <v>41</v>
+      </c>
+      <c r="E59">
+        <v>837</v>
+      </c>
+      <c r="G59" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>44715.759432870371</v>
+      </c>
+      <c r="B60" t="s">
+        <v>9</v>
+      </c>
+      <c r="C60" t="s">
+        <v>42</v>
+      </c>
+      <c r="E60">
+        <v>3</v>
+      </c>
+      <c r="G60" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>44715.759432870371</v>
+      </c>
+      <c r="B61" t="s">
+        <v>9</v>
+      </c>
+      <c r="C61" t="s">
+        <v>43</v>
+      </c>
+      <c r="E61">
+        <v>458</v>
+      </c>
+      <c r="G61" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>44715.759432870371</v>
+      </c>
+      <c r="B62" t="s">
+        <v>9</v>
+      </c>
+      <c r="C62" t="s">
+        <v>31</v>
+      </c>
+      <c r="E62">
+        <v>456</v>
+      </c>
+      <c r="G62" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>44715.759432870371</v>
+      </c>
+      <c r="B63" t="s">
+        <v>9</v>
+      </c>
+      <c r="C63" t="s">
+        <v>32</v>
+      </c>
+      <c r="E63">
+        <v>898</v>
+      </c>
+      <c r="G63" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>44715.759432870371</v>
+      </c>
+      <c r="B64" t="s">
+        <v>9</v>
+      </c>
+      <c r="C64" t="s">
+        <v>15</v>
+      </c>
+      <c r="E64">
+        <v>8</v>
+      </c>
+      <c r="G64" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>44715.759432870371</v>
+      </c>
+      <c r="B65" t="s">
+        <v>9</v>
+      </c>
+      <c r="C65" t="s">
+        <v>16</v>
+      </c>
+      <c r="E65">
+        <v>76</v>
+      </c>
+      <c r="G65" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>44715.759432870371</v>
+      </c>
+      <c r="B66" t="s">
+        <v>9</v>
+      </c>
+      <c r="C66" t="s">
+        <v>19</v>
+      </c>
+      <c r="E66">
+        <v>23</v>
+      </c>
+      <c r="G66" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>44715.759432870371</v>
+      </c>
+      <c r="B67" t="s">
+        <v>9</v>
+      </c>
+      <c r="C67" t="s">
+        <v>20</v>
+      </c>
+      <c r="E67">
+        <v>234</v>
+      </c>
+      <c r="G67" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>44715.759432870371</v>
+      </c>
+      <c r="B68" t="s">
+        <v>9</v>
+      </c>
+      <c r="C68" t="s">
+        <v>23</v>
+      </c>
+      <c r="E68">
+        <v>89</v>
+      </c>
+      <c r="G68" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>44715.759432870371</v>
+      </c>
+      <c r="B69" t="s">
+        <v>9</v>
+      </c>
+      <c r="C69" t="s">
+        <v>24</v>
+      </c>
+      <c r="E69">
+        <v>78</v>
+      </c>
+      <c r="G69" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>44715.759421296294</v>
+      </c>
+      <c r="B70" t="s">
+        <v>9</v>
+      </c>
+      <c r="C70" t="s">
+        <v>27</v>
+      </c>
+      <c r="E70">
+        <v>234</v>
+      </c>
+      <c r="G70" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>44715.759421296294</v>
+      </c>
+      <c r="B71" t="s">
+        <v>9</v>
+      </c>
+      <c r="C71" t="s">
+        <v>28</v>
+      </c>
+      <c r="E71">
+        <v>87</v>
+      </c>
+      <c r="G71" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>44715.759421296294</v>
+      </c>
+      <c r="B72" t="s">
+        <v>9</v>
+      </c>
+      <c r="C72" t="s">
+        <v>10</v>
+      </c>
+      <c r="E72">
+        <v>7383783</v>
+      </c>
+      <c r="G72" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>44715.759421296294</v>
+      </c>
+      <c r="B73" t="s">
+        <v>9</v>
+      </c>
+      <c r="C73" t="s">
+        <v>11</v>
+      </c>
+      <c r="E73">
+        <v>34</v>
+      </c>
+      <c r="G73" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>44715.759421296294</v>
+      </c>
+      <c r="B74" t="s">
+        <v>9</v>
+      </c>
+      <c r="C74" t="s">
+        <v>12</v>
+      </c>
+      <c r="E74">
+        <v>342</v>
+      </c>
+      <c r="G74" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>44715.759421296294</v>
+      </c>
+      <c r="B75" t="s">
+        <v>7</v>
+      </c>
+      <c r="C75" t="s">
+        <v>44</v>
+      </c>
+      <c r="E75">
+        <v>53</v>
+      </c>
+      <c r="G75" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>44715.759421296294</v>
+      </c>
+      <c r="B76" t="s">
+        <v>7</v>
+      </c>
+      <c r="C76" t="s">
+        <v>45</v>
+      </c>
+      <c r="E76">
+        <v>5</v>
+      </c>
+      <c r="G76" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>44715.759421296294</v>
+      </c>
+      <c r="B77" t="s">
+        <v>7</v>
+      </c>
+      <c r="C77" t="s">
+        <v>40</v>
+      </c>
+      <c r="E77">
+        <v>81</v>
+      </c>
+      <c r="G77" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>44715.759421296294</v>
+      </c>
+      <c r="B78" t="s">
+        <v>7</v>
+      </c>
+      <c r="C78" t="s">
+        <v>41</v>
+      </c>
+      <c r="E78">
+        <v>837</v>
+      </c>
+      <c r="G78" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>44715.759421296294</v>
+      </c>
+      <c r="B79" t="s">
+        <v>7</v>
+      </c>
+      <c r="C79" t="s">
+        <v>46</v>
+      </c>
+      <c r="E79">
+        <v>3906</v>
+      </c>
+      <c r="G79" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>44715.759421296294</v>
+      </c>
+      <c r="B80" t="s">
+        <v>7</v>
+      </c>
+      <c r="C80" t="s">
+        <v>47</v>
+      </c>
+      <c r="E80">
+        <v>38</v>
+      </c>
+      <c r="G80" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>44715.759421296294</v>
+      </c>
+      <c r="B81" t="s">
+        <v>7</v>
+      </c>
+      <c r="C81" t="s">
+        <v>42</v>
+      </c>
+      <c r="E81">
+        <v>3</v>
+      </c>
+      <c r="G81" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>44715.759421296294</v>
+      </c>
+      <c r="B82" t="s">
+        <v>7</v>
+      </c>
+      <c r="C82" t="s">
+        <v>43</v>
+      </c>
+      <c r="E82">
+        <v>458</v>
+      </c>
+      <c r="G82" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>44715.759421296294</v>
+      </c>
+      <c r="B83" t="s">
+        <v>7</v>
+      </c>
+      <c r="C83" t="s">
+        <v>29</v>
+      </c>
+      <c r="E83">
+        <v>37</v>
+      </c>
+      <c r="G83" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>44715.759421296294</v>
+      </c>
+      <c r="B84" t="s">
+        <v>7</v>
+      </c>
+      <c r="C84" t="s">
+        <v>30</v>
+      </c>
+      <c r="E84">
+        <v>7</v>
+      </c>
+      <c r="G84" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>44715.759421296294</v>
+      </c>
+      <c r="B85" t="s">
+        <v>7</v>
+      </c>
+      <c r="C85" t="s">
+        <v>31</v>
+      </c>
+      <c r="E85">
+        <v>456</v>
+      </c>
+      <c r="G85" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>44715.759421296294</v>
+      </c>
+      <c r="B86" t="s">
+        <v>7</v>
+      </c>
+      <c r="C86" t="s">
+        <v>32</v>
+      </c>
+      <c r="E86">
+        <v>898</v>
+      </c>
+      <c r="G86" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>44715.759421296294</v>
+      </c>
+      <c r="B87" t="s">
+        <v>7</v>
+      </c>
+      <c r="C87" t="s">
+        <v>13</v>
+      </c>
+      <c r="E87">
+        <v>2432</v>
+      </c>
+      <c r="G87" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>44715.759421296294</v>
+      </c>
+      <c r="B88" t="s">
+        <v>7</v>
+      </c>
+      <c r="C88" t="s">
+        <v>14</v>
+      </c>
+      <c r="E88">
+        <v>79</v>
+      </c>
+      <c r="G88" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>44715.759421296294</v>
+      </c>
+      <c r="B89" t="s">
+        <v>7</v>
+      </c>
+      <c r="C89" t="s">
+        <v>15</v>
+      </c>
+      <c r="E89">
+        <v>8</v>
+      </c>
+      <c r="G89" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>44715.759421296294</v>
+      </c>
+      <c r="B90" t="s">
+        <v>7</v>
+      </c>
+      <c r="C90" t="s">
+        <v>16</v>
+      </c>
+      <c r="E90">
+        <v>76</v>
+      </c>
+      <c r="G90" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>44715.759421296294</v>
+      </c>
+      <c r="B91" t="s">
+        <v>7</v>
+      </c>
+      <c r="C91" t="s">
+        <v>17</v>
+      </c>
+      <c r="E91">
+        <v>56</v>
+      </c>
+      <c r="G91" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>44715.759421296294</v>
+      </c>
+      <c r="B92" t="s">
+        <v>7</v>
+      </c>
+      <c r="C92" t="s">
+        <v>18</v>
+      </c>
+      <c r="E92">
+        <v>3838</v>
+      </c>
+      <c r="G92" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>44715.759409722225</v>
+      </c>
+      <c r="B93" t="s">
+        <v>7</v>
+      </c>
+      <c r="C93" t="s">
+        <v>19</v>
+      </c>
+      <c r="E93">
+        <v>23</v>
+      </c>
+      <c r="G93" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>44715.759409722225</v>
+      </c>
+      <c r="B94" t="s">
+        <v>7</v>
+      </c>
+      <c r="C94" t="s">
+        <v>20</v>
+      </c>
+      <c r="E94">
+        <v>234</v>
+      </c>
+      <c r="G94" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>44715.759409722225</v>
+      </c>
+      <c r="B95" t="s">
+        <v>7</v>
+      </c>
+      <c r="C95" t="s">
+        <v>21</v>
+      </c>
+      <c r="E95">
+        <v>5654</v>
+      </c>
+      <c r="G95" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>44715.759409722225</v>
+      </c>
+      <c r="B96" t="s">
+        <v>7</v>
+      </c>
+      <c r="C96" t="s">
+        <v>22</v>
+      </c>
+      <c r="E96">
+        <v>23</v>
+      </c>
+      <c r="G96" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>44715.759409722225</v>
+      </c>
+      <c r="B97" t="s">
+        <v>7</v>
+      </c>
+      <c r="C97" t="s">
+        <v>23</v>
+      </c>
+      <c r="E97">
+        <v>89</v>
+      </c>
+      <c r="G97" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>44715.759409722225</v>
+      </c>
+      <c r="B98" t="s">
+        <v>7</v>
+      </c>
+      <c r="C98" t="s">
+        <v>24</v>
+      </c>
+      <c r="E98">
+        <v>78</v>
+      </c>
+      <c r="G98" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>44715.759409722225</v>
+      </c>
+      <c r="B99" t="s">
+        <v>7</v>
+      </c>
+      <c r="C99" t="s">
+        <v>25</v>
+      </c>
+      <c r="E99">
+        <v>4789</v>
+      </c>
+      <c r="G99" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>44715.759409722225</v>
+      </c>
+      <c r="B100" t="s">
+        <v>7</v>
+      </c>
+      <c r="C100" t="s">
+        <v>26</v>
+      </c>
+      <c r="E100">
+        <v>12</v>
+      </c>
+      <c r="G100" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>44715.759409722225</v>
+      </c>
+      <c r="B101" t="s">
+        <v>7</v>
+      </c>
+      <c r="C101" t="s">
+        <v>27</v>
+      </c>
+      <c r="E101">
+        <v>234</v>
+      </c>
+      <c r="G101" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>44715.759409722225</v>
+      </c>
+      <c r="B102" t="s">
+        <v>7</v>
+      </c>
+      <c r="C102" t="s">
+        <v>28</v>
+      </c>
+      <c r="E102">
+        <v>87</v>
+      </c>
+      <c r="G102" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>44715.759409722225</v>
+      </c>
+      <c r="B103" t="s">
+        <v>7</v>
+      </c>
+      <c r="C103" t="s">
+        <v>8</v>
+      </c>
+      <c r="E103">
+        <v>546</v>
+      </c>
+      <c r="G103" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>44715.759409722225</v>
+      </c>
+      <c r="B104" t="s">
+        <v>7</v>
+      </c>
+      <c r="C104" t="s">
+        <v>10</v>
+      </c>
+      <c r="E104">
+        <v>77</v>
+      </c>
+      <c r="G104" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <v>44715.759409722225</v>
+      </c>
+      <c r="B105" t="s">
+        <v>7</v>
+      </c>
+      <c r="C105" t="s">
+        <v>11</v>
+      </c>
+      <c r="E105">
+        <v>34</v>
+      </c>
+      <c r="G105" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A106">
+        <v>44715.759409722225</v>
+      </c>
+      <c r="B106" t="s">
+        <v>7</v>
+      </c>
+      <c r="C106" t="s">
+        <v>12</v>
+      </c>
+      <c r="E106">
+        <v>342</v>
+      </c>
+      <c r="G106" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>